<commit_message>
Suossjavri parameter file updated to include information about lateral interactions in the header.
</commit_message>
<xml_diff>
--- a/results/peat_suossjavri/peat_suossjavri.xlsx
+++ b/results/peat_suossjavri/peat_suossjavri.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\work\CryoGrid2020_27\results\peat_suossjavri\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\thin\02_Code\Matlab\CryoGRID\202008_CryoGrid_NewOOP_GIT - CURRENT_THIN\results\peat_suossjavri\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="154">
   <si>
     <t xml:space="preserve">    </t>
   </si>
@@ -471,6 +471,21 @@
   </si>
   <si>
     <t>GROUND_freezeC_bucketW_seb_snow</t>
+  </si>
+  <si>
+    <t>lateral_interactions</t>
+  </si>
+  <si>
+    <t>LIST</t>
+  </si>
+  <si>
+    <t>LAT_WATER_RESERVOIR</t>
+  </si>
+  <si>
+    <t>LAT_REMOVE_SURFACE_WATER</t>
+  </si>
+  <si>
+    <t>END</t>
   </si>
 </sst>
 </file>
@@ -813,23 +828,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F285"/>
+  <dimension ref="A1:F286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.85546875" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="2" max="6" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -837,13 +848,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>121</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -851,7 +862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -862,7 +873,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -873,7 +884,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>129</v>
       </c>
@@ -884,7 +895,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>132</v>
       </c>
@@ -895,7 +906,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>135</v>
       </c>
@@ -909,7 +920,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>137</v>
       </c>
@@ -923,7 +934,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>139</v>
       </c>
@@ -937,7 +948,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>141</v>
       </c>
@@ -951,7 +962,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>143</v>
       </c>
@@ -965,7 +976,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>145</v>
       </c>
@@ -979,134 +990,137 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" t="s">
+        <v>151</v>
+      </c>
+      <c r="D14" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>16</v>
-      </c>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19">
-        <v>0.25</v>
-      </c>
-      <c r="C19" t="s">
-        <v>74</v>
+      <c r="B19" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" t="s">
-        <v>75</v>
+        <v>71</v>
+      </c>
+      <c r="B20">
+        <v>0.25</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>73</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
+        <v>72</v>
+      </c>
+      <c r="B21" t="s">
+        <v>75</v>
       </c>
       <c r="C21" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" t="s">
-        <v>120</v>
+      <c r="B28" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="D30" t="s">
-        <v>67</v>
+        <v>51</v>
+      </c>
+      <c r="B30" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>56</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B31" s="5"/>
       <c r="D31" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32">
-        <v>0.2</v>
-      </c>
-      <c r="C32" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="D32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33">
         <v>0.2</v>
@@ -1115,303 +1129,297 @@
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B34">
-        <v>70</v>
+        <v>0.2</v>
       </c>
       <c r="C34" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C35" t="s">
         <v>38</v>
       </c>
+      <c r="D35" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B36">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B37">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="B38">
-        <v>0.05</v>
+        <v>100</v>
       </c>
       <c r="C38" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>0.05</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B44" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="B45" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>6</v>
-      </c>
-      <c r="B47" t="s">
-        <v>6</v>
-      </c>
-      <c r="C47" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>0</v>
-      </c>
-      <c r="B49">
-        <v>0.05</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B50">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C50">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>0.1</v>
+      </c>
+      <c r="C51">
         <v>2</v>
-      </c>
-      <c r="B51">
-        <v>0.2</v>
-      </c>
-      <c r="C51">
-        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
+        <v>2</v>
+      </c>
+      <c r="B52">
+        <v>0.2</v>
+      </c>
+      <c r="C52">
         <v>10</v>
-      </c>
-      <c r="B52">
-        <v>0.5</v>
-      </c>
-      <c r="C52">
-        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
+        <v>10</v>
+      </c>
+      <c r="B53">
+        <v>0.5</v>
+      </c>
+      <c r="C53">
         <v>20</v>
       </c>
-      <c r="B53">
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>20</v>
+      </c>
+      <c r="B54">
         <v>5</v>
       </c>
-      <c r="C53">
+      <c r="C54">
         <v>100</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D58" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D59" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
+      <c r="B60" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B62" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C62" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D62" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E62" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F61" s="3" t="s">
+      <c r="F62" s="3" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>6</v>
-      </c>
-      <c r="B62" t="s">
-        <v>5</v>
-      </c>
-      <c r="C62" t="s">
-        <v>5</v>
-      </c>
-      <c r="D62" t="s">
-        <v>5</v>
-      </c>
-      <c r="E62" t="s">
-        <v>5</v>
-      </c>
-      <c r="F62" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F63" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>0</v>
-      </c>
-      <c r="B64">
-        <v>0.2</v>
-      </c>
-      <c r="C64">
-        <v>0.5</v>
-      </c>
-      <c r="D64">
-        <v>0</v>
-      </c>
-      <c r="E64">
-        <v>0.3</v>
-      </c>
-      <c r="F64">
-        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B65">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="C65">
         <v>0.5</v>
@@ -1423,12 +1431,12 @@
         <v>0.3</v>
       </c>
       <c r="F65">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B66">
         <v>0.5</v>
@@ -1443,169 +1451,181 @@
         <v>0.3</v>
       </c>
       <c r="F66">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>35</v>
+      <c r="A67">
+        <v>12</v>
+      </c>
+      <c r="B67">
+        <v>0.5</v>
+      </c>
+      <c r="C67">
+        <v>0.5</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0.3</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B72" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
+      <c r="B73" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B75" t="s">
         <v>90</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C75" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>0</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C77">
-        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
+        <v>0</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79">
         <v>10</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B79" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="C79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>35</v>
       </c>
-      <c r="B79" s="4"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B80" s="4"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>109</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C81" s="8"/>
+      <c r="B81" s="4"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>92</v>
-      </c>
-      <c r="B82" s="4">
-        <v>1</v>
+        <v>109</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>119</v>
       </c>
       <c r="C82" s="8"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>92</v>
+      </c>
+      <c r="B83" s="4">
+        <v>1</v>
+      </c>
+      <c r="C83" s="8"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E86" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E87" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B87" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
+      <c r="B88" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B90" s="3" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>6</v>
-      </c>
-      <c r="B90" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>6</v>
+      </c>
+      <c r="B91" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>0</v>
-      </c>
-      <c r="B92">
-        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B93">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B94">
         <v>-1</v>
@@ -1613,174 +1633,173 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="B95">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
+        <v>100</v>
+      </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97">
         <v>5000</v>
       </c>
-      <c r="B96">
+      <c r="B97">
         <v>20</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B101" s="6"/>
-      <c r="C101" s="6"/>
-    </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+      <c r="B102" s="6"/>
+      <c r="C102" s="6"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B103" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C103" s="6"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C104" s="6"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B104" s="7">
-        <v>1</v>
-      </c>
-      <c r="C104" s="6"/>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B105" s="6"/>
+      <c r="B105" s="7">
+        <v>1</v>
+      </c>
       <c r="C105" s="6"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B106" s="6" t="s">
+      <c r="B106" s="6"/>
+      <c r="C106" s="6"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B107" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C106" s="6" t="s">
+      <c r="C107" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D107" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>1</v>
-      </c>
-      <c r="B107" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="C107" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="D107" t="s">
-        <v>5</v>
-      </c>
-      <c r="E107" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B108" s="6">
-        <v>0.99</v>
+        <v>0.15</v>
       </c>
       <c r="C108" s="6">
-        <v>0.99</v>
+        <v>0.15</v>
       </c>
       <c r="D108" t="s">
         <v>5</v>
       </c>
       <c r="E108" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B109" s="6">
-        <v>1E-3</v>
+        <v>0.99</v>
       </c>
       <c r="C109" s="6">
-        <v>1E-3</v>
+        <v>0.99</v>
       </c>
       <c r="D109" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E109" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="B110" s="6">
-        <v>100</v>
-      </c>
-      <c r="C110" s="6"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C110" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="D110" t="s">
+        <v>6</v>
+      </c>
+      <c r="E110" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>89</v>
+      </c>
+      <c r="B111" s="6">
+        <v>100</v>
+      </c>
+      <c r="C111" s="6"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>86</v>
       </c>
-      <c r="B111" s="6">
-        <v>1</v>
-      </c>
-      <c r="C111" s="6">
-        <v>1</v>
-      </c>
-      <c r="D111" t="s">
+      <c r="B112" s="6">
+        <v>1</v>
+      </c>
+      <c r="C112" s="6">
+        <v>1</v>
+      </c>
+      <c r="D112" t="s">
         <v>87</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E112" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B112" s="6"/>
-      <c r="C112" s="6"/>
-    </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>93</v>
-      </c>
-      <c r="B113" s="9">
-        <v>1.0000000000000001E-5</v>
-      </c>
+      <c r="B113" s="6"/>
       <c r="C113" s="6"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>94</v>
-      </c>
-      <c r="B114">
-        <v>0.1</v>
+        <v>93</v>
+      </c>
+      <c r="B114" s="9">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="C114" s="6"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B115">
         <v>0.1</v>
@@ -1789,29 +1808,29 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
+        <v>95</v>
+      </c>
+      <c r="B116">
+        <v>0.1</v>
+      </c>
+      <c r="C116" s="6"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>96</v>
       </c>
-      <c r="B116">
+      <c r="B117">
         <v>0.5</v>
       </c>
-      <c r="C116" s="6"/>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B117" s="6"/>
       <c r="C117" s="6"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>103</v>
-      </c>
-      <c r="B118" s="6">
-        <v>1000</v>
-      </c>
+      <c r="B118" s="6"/>
       <c r="C118" s="6"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B119" s="6">
         <v>1000</v>
@@ -1820,713 +1839,718 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B120" s="6">
-        <v>-40</v>
-      </c>
-      <c r="C120" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E120" t="s">
-        <v>0</v>
-      </c>
+        <v>1000</v>
+      </c>
+      <c r="C120" s="6"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B121" s="6">
-        <v>0.05</v>
-      </c>
-      <c r="C121" s="6">
-        <v>3600</v>
-      </c>
-      <c r="D121" t="s">
-        <v>7</v>
+        <v>-40</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>0</v>
       </c>
       <c r="E121" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B122" s="6">
-        <v>0.97</v>
+        <v>0.05</v>
       </c>
       <c r="C122" s="6">
-        <v>50000</v>
+        <v>3600</v>
       </c>
       <c r="D122" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E122" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B123" s="6">
-        <v>0.03</v>
-      </c>
-      <c r="C123" s="6"/>
+        <v>0.97</v>
+      </c>
+      <c r="C123" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D123" t="s">
+        <v>8</v>
+      </c>
+      <c r="E123" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>0</v>
-      </c>
-      <c r="B124" s="6" t="s">
-        <v>0</v>
+        <v>108</v>
+      </c>
+      <c r="B124" s="6">
+        <v>0.03</v>
       </c>
       <c r="C124" s="6"/>
-      <c r="E124" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>64</v>
-      </c>
-      <c r="B125" s="6">
-        <v>3600</v>
+        <v>0</v>
+      </c>
+      <c r="B125" s="6" t="s">
+        <v>0</v>
       </c>
       <c r="C125" s="6"/>
+      <c r="E125" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B126" s="6">
-        <v>50000</v>
+        <v>3600</v>
       </c>
       <c r="C126" s="6"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
+        <v>65</v>
+      </c>
+      <c r="B127" s="6">
+        <v>50000</v>
+      </c>
+      <c r="C127" s="6"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>111</v>
       </c>
-      <c r="B127" s="6">
+      <c r="B128" s="6">
         <v>0.01</v>
       </c>
-      <c r="C127" s="6"/>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B128" s="6"/>
+      <c r="C128" s="6"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>83</v>
-      </c>
-      <c r="B129" s="6">
-        <v>3</v>
-      </c>
-      <c r="C129" s="6"/>
+      <c r="B129" s="6"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>83</v>
+      </c>
+      <c r="B130" s="6">
+        <v>3</v>
+      </c>
+      <c r="C130" s="6"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>43</v>
       </c>
-      <c r="B130" s="6"/>
-      <c r="C130" s="6"/>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
+      <c r="B131" s="6"/>
+      <c r="C131" s="6"/>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C132" s="6" t="s">
+      <c r="C133" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D132" t="s">
+      <c r="D133" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B133" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C133" s="6"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C134" s="6"/>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B134" s="7">
-        <v>1</v>
-      </c>
-      <c r="C134" s="6"/>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B135" s="6"/>
+      <c r="B135" s="7">
+        <v>1</v>
+      </c>
       <c r="C135" s="6"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B136" s="6" t="s">
+      <c r="B136" s="6"/>
+      <c r="C136" s="6"/>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B137" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C136" s="6">
+      <c r="C137" s="6">
         <v>0.99</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D137" t="s">
         <v>5</v>
       </c>
-      <c r="E136" t="s">
+      <c r="E137" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>98</v>
-      </c>
-      <c r="B137" s="6">
-        <v>0</v>
-      </c>
-      <c r="C137" s="6">
-        <v>1E-3</v>
-      </c>
-      <c r="D137" t="s">
-        <v>6</v>
-      </c>
-      <c r="E137" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B138" s="6">
-        <v>0.71</v>
-      </c>
-      <c r="C138" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="C138" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="D138" t="s">
+        <v>6</v>
+      </c>
+      <c r="E138" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B139" s="6">
-        <v>0.21</v>
+        <v>0.71</v>
       </c>
       <c r="C139" s="6"/>
-      <c r="D139" t="s">
-        <v>102</v>
-      </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="B140" s="6">
-        <v>0.99</v>
+        <v>0.21</v>
       </c>
       <c r="C140" s="6"/>
+      <c r="D140" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B141" s="6">
-        <v>1E-3</v>
+        <v>0.99</v>
       </c>
       <c r="C141" s="6"/>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="B142" s="6">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="C142" s="6"/>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B143" s="6">
-        <v>48</v>
-      </c>
-      <c r="C143" s="6">
-        <v>3600</v>
-      </c>
-      <c r="D143" t="s">
-        <v>7</v>
-      </c>
-      <c r="E143" t="s">
-        <v>13</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C143" s="6"/>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>101</v>
+      </c>
+      <c r="B144" s="6">
         <v>48</v>
       </c>
-      <c r="B144" s="6">
-        <v>0.05</v>
-      </c>
       <c r="C144" s="6">
-        <v>50000</v>
+        <v>3600</v>
       </c>
       <c r="D144" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E144" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>93</v>
-      </c>
-      <c r="B145" s="9">
-        <v>1E-4</v>
-      </c>
-      <c r="C145" s="6"/>
+        <v>48</v>
+      </c>
+      <c r="B145" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="C145" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D145" t="s">
+        <v>8</v>
+      </c>
+      <c r="E145" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>97</v>
-      </c>
-      <c r="B146" s="6">
-        <v>0.02</v>
+        <v>93</v>
+      </c>
+      <c r="B146" s="9">
+        <v>1E-4</v>
       </c>
       <c r="C146" s="6"/>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="B147" s="6">
-        <v>3600</v>
+        <v>0.02</v>
       </c>
       <c r="C147" s="6"/>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
+        <v>64</v>
+      </c>
+      <c r="B148" s="6">
+        <v>3600</v>
+      </c>
+      <c r="C148" s="6"/>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>65</v>
       </c>
-      <c r="B148" s="6">
+      <c r="B149" s="6">
         <v>50000</v>
       </c>
-      <c r="C148" s="6"/>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B149" s="6"/>
       <c r="C149" s="6"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>43</v>
-      </c>
       <c r="B150" s="6"/>
       <c r="C150" s="6"/>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>43</v>
+      </c>
+      <c r="B151" s="6"/>
       <c r="C151" s="6"/>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A152" s="1"/>
+      <c r="C152" s="6"/>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A153" s="1" t="s">
+      <c r="A153" s="1"/>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A154" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B154" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B155" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B155" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B156" s="6"/>
+      <c r="B156" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B157" s="6" t="s">
+      <c r="B157" s="6"/>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B158" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C157" s="6" t="s">
+      <c r="C158" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D157" t="s">
+      <c r="D158" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>1</v>
-      </c>
-      <c r="B158" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="C158" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="D158" t="s">
-        <v>5</v>
-      </c>
-      <c r="E158" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B159" s="6">
-        <v>0.99</v>
+        <v>0.15</v>
       </c>
       <c r="C159" s="6">
-        <v>0.99</v>
+        <v>0.15</v>
       </c>
       <c r="D159" t="s">
         <v>5</v>
       </c>
       <c r="E159" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B160" s="6">
-        <v>1E-3</v>
+        <v>0.99</v>
       </c>
       <c r="C160" s="6">
-        <v>1E-3</v>
+        <v>0.99</v>
       </c>
       <c r="D160" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E160" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="B161" s="6">
-        <v>100</v>
-      </c>
-      <c r="C161" s="6"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C161" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="D161" t="s">
+        <v>6</v>
+      </c>
+      <c r="E161" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B162" s="6">
-        <v>10</v>
-      </c>
-      <c r="C162" s="6">
-        <v>1</v>
-      </c>
-      <c r="D162" t="s">
-        <v>87</v>
-      </c>
-      <c r="E162" t="s">
-        <v>88</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C162" s="6"/>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>0</v>
-      </c>
-      <c r="B163" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C163" s="6" t="s">
-        <v>0</v>
+        <v>86</v>
+      </c>
+      <c r="B163" s="6">
+        <v>10</v>
+      </c>
+      <c r="C163" s="6">
+        <v>1</v>
+      </c>
+      <c r="D163" t="s">
+        <v>87</v>
       </c>
       <c r="E163" t="s">
-        <v>0</v>
+        <v>88</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>64</v>
-      </c>
-      <c r="B164" s="6">
-        <v>3600</v>
-      </c>
-      <c r="C164" s="6">
-        <v>3600</v>
-      </c>
-      <c r="D164" t="s">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="B164" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C164" s="6" t="s">
+        <v>0</v>
       </c>
       <c r="E164" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
+        <v>64</v>
+      </c>
+      <c r="B165" s="6">
+        <v>3600</v>
+      </c>
+      <c r="C165" s="6">
+        <v>3600</v>
+      </c>
+      <c r="D165" t="s">
+        <v>7</v>
+      </c>
+      <c r="E165" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>65</v>
       </c>
-      <c r="B165" s="6">
+      <c r="B166" s="6">
         <v>50000</v>
       </c>
-      <c r="C165" s="6">
+      <c r="C166" s="6">
         <v>50000</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D166" t="s">
         <v>8</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E166" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B166" s="6"/>
-      <c r="C166" s="6"/>
-    </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>83</v>
-      </c>
-      <c r="B167" s="6">
-        <v>3</v>
-      </c>
+      <c r="B167" s="6"/>
       <c r="C167" s="6"/>
-      <c r="E167" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
+        <v>83</v>
+      </c>
+      <c r="B168" s="6">
+        <v>3</v>
+      </c>
+      <c r="C168" s="6"/>
+      <c r="E168" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>43</v>
       </c>
-      <c r="B168" s="6"/>
-      <c r="C168" s="6"/>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B169" s="6"/>
+      <c r="C169" s="6"/>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B170" s="6"/>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A171" s="1" t="s">
+      <c r="B171" s="6"/>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A172" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B172" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B173" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B173" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B174" s="6"/>
+      <c r="B174" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B175" s="6" t="s">
+      <c r="B175" s="6"/>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B176" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C175" s="6" t="s">
+      <c r="C176" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D176" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>1</v>
-      </c>
-      <c r="B176" s="6">
-        <v>0.08</v>
-      </c>
-      <c r="C176" s="6">
-        <v>0.08</v>
-      </c>
-      <c r="D176" t="s">
-        <v>5</v>
-      </c>
-      <c r="E176" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>113</v>
+        <v>1</v>
       </c>
       <c r="B177" s="6">
-        <v>2</v>
-      </c>
-      <c r="C177" s="6" t="s">
-        <v>114</v>
+        <v>0.08</v>
+      </c>
+      <c r="C177" s="6">
+        <v>0.08</v>
       </c>
       <c r="D177" t="s">
-        <v>115</v>
+        <v>5</v>
       </c>
       <c r="E177" t="s">
-        <v>116</v>
+        <v>9</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
+        <v>113</v>
+      </c>
+      <c r="B178" s="6">
         <v>2</v>
       </c>
-      <c r="B178" s="6">
-        <v>0.99</v>
-      </c>
-      <c r="C178" s="6">
-        <v>0.99</v>
+      <c r="C178" s="6" t="s">
+        <v>114</v>
       </c>
       <c r="D178" t="s">
-        <v>5</v>
+        <v>115</v>
       </c>
       <c r="E178" t="s">
-        <v>10</v>
+        <v>116</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B179" s="6">
-        <v>1E-3</v>
+        <v>0.99</v>
       </c>
       <c r="C179" s="6">
-        <v>1E-3</v>
+        <v>0.99</v>
       </c>
       <c r="D179" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E179" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="B180" s="6">
-        <v>0</v>
-      </c>
-      <c r="C180" s="6"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C180" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="D180" t="s">
+        <v>6</v>
+      </c>
+      <c r="E180" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B181" s="6">
-        <v>10</v>
-      </c>
-      <c r="C181" s="6">
-        <v>1</v>
-      </c>
-      <c r="D181" t="s">
-        <v>87</v>
-      </c>
-      <c r="E181" t="s">
-        <v>88</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C181" s="6"/>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>0</v>
-      </c>
-      <c r="B182" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C182" s="6" t="s">
-        <v>0</v>
+        <v>86</v>
+      </c>
+      <c r="B182" s="6">
+        <v>10</v>
+      </c>
+      <c r="C182" s="6">
+        <v>1</v>
+      </c>
+      <c r="D182" t="s">
+        <v>87</v>
       </c>
       <c r="E182" t="s">
-        <v>0</v>
+        <v>88</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>64</v>
-      </c>
-      <c r="B183" s="6">
-        <v>3600</v>
-      </c>
-      <c r="C183" s="6">
-        <v>3600</v>
-      </c>
-      <c r="D183" t="s">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="B183" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C183" s="6" t="s">
+        <v>0</v>
       </c>
       <c r="E183" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
+        <v>64</v>
+      </c>
+      <c r="B184" s="6">
+        <v>3600</v>
+      </c>
+      <c r="C184" s="6">
+        <v>3600</v>
+      </c>
+      <c r="D184" t="s">
+        <v>7</v>
+      </c>
+      <c r="E184" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
         <v>65</v>
       </c>
-      <c r="B184" s="6">
+      <c r="B185" s="6">
         <v>50000</v>
       </c>
-      <c r="C184" s="6">
+      <c r="C185" s="6">
         <v>50000</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D185" t="s">
         <v>8</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E185" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B185" s="6"/>
-      <c r="C185" s="6"/>
-    </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>117</v>
-      </c>
-      <c r="B186" s="4" t="s">
-        <v>118</v>
-      </c>
+      <c r="B186" s="6"/>
       <c r="C186" s="6"/>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
+        <v>117</v>
+      </c>
+      <c r="B187" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C187" s="6"/>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
         <v>43</v>
       </c>
-      <c r="B187" s="6"/>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B188" s="6"/>
-      <c r="C188" s="6"/>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B189" s="9"/>
+      <c r="B189" s="6"/>
       <c r="C189" s="6"/>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B190" s="6"/>
+      <c r="B190" s="9"/>
       <c r="C190" s="6"/>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -2555,27 +2579,26 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B197" s="6"/>
+      <c r="C197" s="6"/>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A198" s="2"/>
+      <c r="B198" s="6"/>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="2"/>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B213" s="9"/>
-    </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A241" s="4"/>
-      <c r="C241" s="6"/>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" s="2"/>
+    </row>
+    <row r="214" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B214" s="9"/>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A242" s="1"/>
+      <c r="A242" s="4"/>
+      <c r="C242" s="6"/>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A243" s="2"/>
-      <c r="B243" s="7"/>
-      <c r="C243" s="6"/>
+      <c r="A243" s="1"/>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" s="2"/>
@@ -2583,7 +2606,8 @@
       <c r="C244" s="6"/>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B245" s="6"/>
+      <c r="A245" s="2"/>
+      <c r="B245" s="7"/>
       <c r="C245" s="6"/>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
@@ -2662,19 +2686,18 @@
       <c r="B264" s="6"/>
       <c r="C264" s="6"/>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B267" s="6"/>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B265" s="6"/>
+      <c r="C265" s="6"/>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B268" s="6"/>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A269" s="1"/>
+      <c r="B269" s="6"/>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A270" s="2"/>
-      <c r="B270" s="7"/>
-      <c r="C270" s="6"/>
+      <c r="A270" s="1"/>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" s="2"/>
@@ -2682,7 +2705,8 @@
       <c r="C271" s="6"/>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B272" s="6"/>
+      <c r="A272" s="2"/>
+      <c r="B272" s="7"/>
       <c r="C272" s="6"/>
     </row>
     <row r="273" spans="2:3" x14ac:dyDescent="0.25">
@@ -2734,7 +2758,11 @@
       <c r="C284" s="6"/>
     </row>
     <row r="285" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B285" s="6"/>
       <c r="C285" s="6"/>
+    </row>
+    <row r="286" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C286" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
UPDATE: Finse_4432 and peat_suossjavri cases updated to be runnable with current version of codebase (GROUND_CLASS, LATERAL_CLASS, IA_CLASS sections added to parameter files). Both cases can be executed with Excel and YAML parameter files. Cases are executable without errors, but calculation results have not been checked for differences.
</commit_message>
<xml_diff>
--- a/results/peat_suossjavri/peat_suossjavri.xlsx
+++ b/results/peat_suossjavri/peat_suossjavri.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="167">
   <si>
     <t xml:space="preserve">    </t>
   </si>
@@ -71,9 +71,6 @@
     <t>maximum change of energy per timestep</t>
   </si>
   <si>
-    <t>CLASS</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -486,6 +483,48 @@
   </si>
   <si>
     <t>END</t>
+  </si>
+  <si>
+    <t>GROUND_CLASS</t>
+  </si>
+  <si>
+    <t>ia_time_increment</t>
+  </si>
+  <si>
+    <t>IA_CLASS</t>
+  </si>
+  <si>
+    <t>reservoir_elevation</t>
+  </si>
+  <si>
+    <t>reservoir_temperature</t>
+  </si>
+  <si>
+    <t>only active for Xice classes - if empty, water added at the temperature of the respective grid cell</t>
+  </si>
+  <si>
+    <t>hardBottom_cutoff</t>
+  </si>
+  <si>
+    <t>hard bottom if saturated and water content below</t>
+  </si>
+  <si>
+    <t>distance_reservoir</t>
+  </si>
+  <si>
+    <t>reservoir_contact_length</t>
+  </si>
+  <si>
+    <t>NO_PARAMERTERS_REQUIRED</t>
+  </si>
+  <si>
+    <t>LATERAL_CLASS</t>
+  </si>
+  <si>
+    <t>LATERAL_IA_1D</t>
+  </si>
+  <si>
+    <t>LATERAL_IA_3D</t>
   </si>
 </sst>
 </file>
@@ -828,10 +867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F286"/>
+  <dimension ref="A1:F285"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A188" workbookViewId="0">
+      <selection activeCell="B224" sqref="B224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,21 +881,21 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
@@ -864,277 +903,271 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" t="s">
         <v>123</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>124</v>
-      </c>
-      <c r="D4" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" t="s">
         <v>126</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>127</v>
-      </c>
-      <c r="D5" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" t="s">
         <v>129</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>130</v>
-      </c>
-      <c r="D6" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" t="s">
         <v>132</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>133</v>
-      </c>
-      <c r="D7" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
         <v>135</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
         <v>137</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
         <v>139</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
         <v>141</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
         <v>143</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
         <v>145</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" t="s">
         <v>149</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>150</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>151</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>152</v>
       </c>
-      <c r="E14" t="s">
-        <v>153</v>
-      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>147</v>
+      <c r="A15" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B15">
+        <v>0.25</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="A16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B19" s="2">
-        <v>1</v>
+        <v>67</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20">
-        <v>0.25</v>
-      </c>
-      <c r="C20" t="s">
-        <v>74</v>
+      <c r="A20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" t="s">
-        <v>75</v>
+        <v>70</v>
+      </c>
+      <c r="B21">
+        <v>0.25</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
+        <v>74</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" t="s">
-        <v>120</v>
+        <v>48</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="D31" t="s">
-        <v>67</v>
+        <v>50</v>
+      </c>
+      <c r="B31" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>56</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="B32" s="5"/>
       <c r="D32" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33">
-        <v>0.2</v>
-      </c>
-      <c r="C33" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B34">
         <v>0.2</v>
@@ -1143,303 +1176,297 @@
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B35">
-        <v>70</v>
+        <v>0.2</v>
       </c>
       <c r="C35" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>70</v>
+      </c>
+      <c r="C36" t="s">
         <v>37</v>
       </c>
-      <c r="B36">
-        <v>10</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="B37">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B38">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C38" t="s">
         <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="B39">
-        <v>0.05</v>
+        <v>100</v>
       </c>
       <c r="C39" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>0.05</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>42</v>
+        <v>65</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>16</v>
+      <c r="A44" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B45" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>6</v>
-      </c>
-      <c r="B48" t="s">
-        <v>6</v>
-      </c>
-      <c r="C48" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>34</v>
+        <v>6</v>
+      </c>
+      <c r="B49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>0</v>
-      </c>
-      <c r="B50">
-        <v>0.05</v>
-      </c>
-      <c r="C50">
-        <v>1</v>
+      <c r="A50" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B51">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>0.1</v>
+      </c>
+      <c r="C52">
         <v>2</v>
-      </c>
-      <c r="B52">
-        <v>0.2</v>
-      </c>
-      <c r="C52">
-        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
+        <v>2</v>
+      </c>
+      <c r="B53">
+        <v>0.2</v>
+      </c>
+      <c r="C53">
         <v>10</v>
-      </c>
-      <c r="B53">
-        <v>0.5</v>
-      </c>
-      <c r="C53">
-        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
+        <v>10</v>
+      </c>
+      <c r="B54">
+        <v>0.5</v>
+      </c>
+      <c r="C54">
         <v>20</v>
       </c>
-      <c r="B54">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>20</v>
+      </c>
+      <c r="B55">
         <v>5</v>
       </c>
-      <c r="C54">
+      <c r="C55">
         <v>100</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D59" t="s">
-        <v>46</v>
+      <c r="A59" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B60" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B61" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F63" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>6</v>
-      </c>
-      <c r="B63" t="s">
-        <v>5</v>
-      </c>
-      <c r="C63" t="s">
-        <v>5</v>
-      </c>
-      <c r="D63" t="s">
-        <v>5</v>
-      </c>
-      <c r="E63" t="s">
-        <v>5</v>
-      </c>
-      <c r="F63" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>34</v>
+        <v>6</v>
+      </c>
+      <c r="B64" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" t="s">
+        <v>5</v>
+      </c>
+      <c r="E64" t="s">
+        <v>5</v>
+      </c>
+      <c r="F64" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>0</v>
-      </c>
-      <c r="B65">
-        <v>0.2</v>
-      </c>
-      <c r="C65">
-        <v>0.5</v>
-      </c>
-      <c r="D65">
-        <v>0</v>
-      </c>
-      <c r="E65">
-        <v>0.3</v>
-      </c>
-      <c r="F65">
-        <v>1</v>
+      <c r="A65" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B66">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="C66">
         <v>0.5</v>
@@ -1451,12 +1478,12 @@
         <v>0.3</v>
       </c>
       <c r="F66">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B67">
         <v>0.5</v>
@@ -1471,169 +1498,181 @@
         <v>0.3</v>
       </c>
       <c r="F67">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>35</v>
+      <c r="A68">
+        <v>12</v>
+      </c>
+      <c r="B68">
+        <v>0.5</v>
+      </c>
+      <c r="C68">
+        <v>0.5</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0.3</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>16</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B73" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B75" t="s">
+        <v>20</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B74" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B76" t="s">
+        <v>89</v>
+      </c>
+      <c r="C76" t="s">
         <v>90</v>
-      </c>
-      <c r="C75" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>0</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C78">
-        <v>1</v>
+      <c r="A78" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
+        <v>0</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80">
         <v>10</v>
       </c>
-      <c r="B79" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>35</v>
-      </c>
-      <c r="B80" s="4"/>
+      <c r="B80" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>34</v>
+      </c>
       <c r="B81" s="4"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>109</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C82" s="8"/>
+      <c r="B82" s="4"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>92</v>
-      </c>
-      <c r="B83" s="4">
-        <v>1</v>
+        <v>108</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>118</v>
       </c>
       <c r="C83" s="8"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E87" t="s">
-        <v>82</v>
+        <v>91</v>
+      </c>
+      <c r="B84" s="4">
+        <v>1</v>
+      </c>
+      <c r="C84" s="8"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B88" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B90" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E88" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="B89" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>6</v>
-      </c>
-      <c r="B91" t="s">
-        <v>28</v>
+      <c r="A91" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>34</v>
+        <v>6</v>
+      </c>
+      <c r="B92" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>0</v>
-      </c>
-      <c r="B93">
-        <v>5</v>
+      <c r="A93" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B94">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B95">
         <v>-1</v>
@@ -1641,174 +1680,173 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="B96">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
+        <v>100</v>
+      </c>
+      <c r="B97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98">
         <v>5000</v>
       </c>
-      <c r="B97">
+      <c r="B98">
         <v>20</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B102" s="6"/>
-      <c r="C102" s="6"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="B103" s="6"/>
+      <c r="C103" s="6"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B104" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C104" s="6"/>
+      <c r="A104" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B105" s="7">
-        <v>1</v>
+        <v>153</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="C105" s="6"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B106" s="6"/>
+      <c r="A106" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B106" s="7">
+        <v>1</v>
+      </c>
       <c r="C106" s="6"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B107" s="6" t="s">
+      <c r="B107" s="6"/>
+      <c r="C107" s="6"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B108" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C108" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C107" s="6" t="s">
+      <c r="D108" t="s">
         <v>18</v>
-      </c>
-      <c r="D107" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>1</v>
-      </c>
-      <c r="B108" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="C108" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="D108" t="s">
-        <v>5</v>
-      </c>
-      <c r="E108" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B109" s="6">
-        <v>0.99</v>
+        <v>0.15</v>
       </c>
       <c r="C109" s="6">
-        <v>0.99</v>
+        <v>0.15</v>
       </c>
       <c r="D109" t="s">
         <v>5</v>
       </c>
       <c r="E109" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B110" s="6">
-        <v>1E-3</v>
+        <v>0.99</v>
       </c>
       <c r="C110" s="6">
-        <v>1E-3</v>
+        <v>0.99</v>
       </c>
       <c r="D110" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E110" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="B111" s="6">
-        <v>100</v>
-      </c>
-      <c r="C111" s="6"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C111" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="D111" t="s">
+        <v>6</v>
+      </c>
+      <c r="E111" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>88</v>
+      </c>
+      <c r="B112" s="6">
+        <v>100</v>
+      </c>
+      <c r="C112" s="6"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>85</v>
+      </c>
+      <c r="B113" s="6">
+        <v>1</v>
+      </c>
+      <c r="C113" s="6">
+        <v>1</v>
+      </c>
+      <c r="D113" t="s">
         <v>86</v>
       </c>
-      <c r="B112" s="6">
-        <v>1</v>
-      </c>
-      <c r="C112" s="6">
-        <v>1</v>
-      </c>
-      <c r="D112" t="s">
+      <c r="E113" t="s">
         <v>87</v>
       </c>
-      <c r="E112" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B113" s="6"/>
-      <c r="C113" s="6"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>93</v>
-      </c>
-      <c r="B114" s="9">
-        <v>1.0000000000000001E-5</v>
-      </c>
+      <c r="B114" s="6"/>
       <c r="C114" s="6"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>94</v>
-      </c>
-      <c r="B115">
-        <v>0.1</v>
+        <v>92</v>
+      </c>
+      <c r="B115" s="9">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="C115" s="6"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B116">
         <v>0.1</v>
@@ -1817,29 +1855,29 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B117">
+        <v>0.1</v>
+      </c>
+      <c r="C117" s="6"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>95</v>
+      </c>
+      <c r="B118">
         <v>0.5</v>
       </c>
-      <c r="C117" s="6"/>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B118" s="6"/>
       <c r="C118" s="6"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>103</v>
-      </c>
-      <c r="B119" s="6">
-        <v>1000</v>
-      </c>
+      <c r="B119" s="6"/>
       <c r="C119" s="6"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B120" s="6">
         <v>1000</v>
@@ -1848,33 +1886,25 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B121" s="6">
-        <v>-40</v>
-      </c>
-      <c r="C121" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E121" t="s">
-        <v>0</v>
-      </c>
+        <v>1000</v>
+      </c>
+      <c r="C121" s="6"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B122" s="6">
-        <v>0.05</v>
-      </c>
-      <c r="C122" s="6">
-        <v>3600</v>
-      </c>
-      <c r="D122" t="s">
-        <v>7</v>
+        <v>-40</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>0</v>
       </c>
       <c r="E122" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -1882,723 +1912,962 @@
         <v>106</v>
       </c>
       <c r="B123" s="6">
-        <v>0.97</v>
+        <v>0.05</v>
       </c>
       <c r="C123" s="6">
-        <v>50000</v>
+        <v>3600</v>
       </c>
       <c r="D123" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E123" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B124" s="6">
-        <v>0.03</v>
-      </c>
-      <c r="C124" s="6"/>
+        <v>0.97</v>
+      </c>
+      <c r="C124" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D124" t="s">
+        <v>8</v>
+      </c>
+      <c r="E124" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>0</v>
-      </c>
-      <c r="B125" s="6" t="s">
-        <v>0</v>
+        <v>107</v>
+      </c>
+      <c r="B125" s="6">
+        <v>0.03</v>
       </c>
       <c r="C125" s="6"/>
-      <c r="E125" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>64</v>
-      </c>
-      <c r="B126" s="6">
-        <v>3600</v>
+        <v>0</v>
+      </c>
+      <c r="B126" s="6" t="s">
+        <v>0</v>
       </c>
       <c r="C126" s="6"/>
+      <c r="E126" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B127" s="6">
-        <v>50000</v>
+        <v>3600</v>
       </c>
       <c r="C127" s="6"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="B128" s="6">
+        <v>50000</v>
+      </c>
+      <c r="C128" s="6"/>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>110</v>
+      </c>
+      <c r="B129" s="6">
         <v>0.01</v>
       </c>
-      <c r="C128" s="6"/>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B129" s="6"/>
+      <c r="C129" s="6"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>83</v>
-      </c>
-      <c r="B130" s="6">
-        <v>3</v>
-      </c>
-      <c r="C130" s="6"/>
+      <c r="B130" s="6"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>43</v>
-      </c>
-      <c r="B131" s="6"/>
+        <v>82</v>
+      </c>
+      <c r="B131" s="6">
+        <v>3</v>
+      </c>
       <c r="C131" s="6"/>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C133" s="6" t="s">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>42</v>
+      </c>
+      <c r="B132" s="6"/>
+      <c r="C132" s="6"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C134" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D134" t="s">
         <v>18</v>
       </c>
-      <c r="D133" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B134" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C134" s="6"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B135" s="7">
-        <v>1</v>
+        <v>153</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="C135" s="6"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B136" s="6"/>
+      <c r="A136" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B136" s="7">
+        <v>1</v>
+      </c>
       <c r="C136" s="6"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B137" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C137" s="6">
+      <c r="B137" s="6"/>
+      <c r="C137" s="6"/>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B138" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C138" s="6">
         <v>0.99</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D138" t="s">
         <v>5</v>
       </c>
-      <c r="E137" t="s">
+      <c r="E138" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>98</v>
-      </c>
-      <c r="B138" s="6">
-        <v>0</v>
-      </c>
-      <c r="C138" s="6">
-        <v>1E-3</v>
-      </c>
-      <c r="D138" t="s">
-        <v>6</v>
-      </c>
-      <c r="E138" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B139" s="6">
-        <v>0.71</v>
-      </c>
-      <c r="C139" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="C139" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="D139" t="s">
+        <v>6</v>
+      </c>
+      <c r="E139" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>99</v>
       </c>
       <c r="B140" s="6">
-        <v>0.21</v>
+        <v>0.71</v>
       </c>
       <c r="C140" s="6"/>
-      <c r="D140" t="s">
-        <v>102</v>
-      </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="B141" s="6">
-        <v>0.99</v>
+        <v>0.21</v>
       </c>
       <c r="C141" s="6"/>
+      <c r="D141" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B142" s="6">
-        <v>1E-3</v>
+        <v>0.99</v>
       </c>
       <c r="C142" s="6"/>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="B143" s="6">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="C143" s="6"/>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="B144" s="6">
-        <v>48</v>
-      </c>
-      <c r="C144" s="6">
-        <v>3600</v>
-      </c>
-      <c r="D144" t="s">
-        <v>7</v>
-      </c>
-      <c r="E144" t="s">
-        <v>13</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C144" s="6"/>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
+        <v>100</v>
+      </c>
+      <c r="B145" s="6">
         <v>48</v>
       </c>
-      <c r="B145" s="6">
-        <v>0.05</v>
-      </c>
       <c r="C145" s="6">
-        <v>50000</v>
+        <v>3600</v>
       </c>
       <c r="D145" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E145" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>93</v>
-      </c>
-      <c r="B146" s="9">
-        <v>1E-4</v>
-      </c>
-      <c r="C146" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="B146" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="C146" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D146" t="s">
+        <v>8</v>
+      </c>
+      <c r="E146" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>97</v>
-      </c>
-      <c r="B147" s="6">
-        <v>0.02</v>
+        <v>92</v>
+      </c>
+      <c r="B147" s="9">
+        <v>1E-4</v>
       </c>
       <c r="C147" s="6"/>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="B148" s="6">
-        <v>3600</v>
+        <v>0.02</v>
       </c>
       <c r="C148" s="6"/>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B149" s="6">
+        <v>3600</v>
+      </c>
+      <c r="C149" s="6"/>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>64</v>
+      </c>
+      <c r="B150" s="6">
         <v>50000</v>
       </c>
-      <c r="C149" s="6"/>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B150" s="6"/>
       <c r="C150" s="6"/>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>43</v>
-      </c>
       <c r="B151" s="6"/>
       <c r="C151" s="6"/>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>42</v>
+      </c>
+      <c r="B152" s="6"/>
       <c r="C152" s="6"/>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A153" s="1"/>
+      <c r="C153" s="6"/>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A154" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A154" s="1"/>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A155" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B155" s="7" t="s">
-        <v>16</v>
+      <c r="A155" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B156" s="7">
-        <v>1</v>
+        <v>153</v>
+      </c>
+      <c r="B156" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B157" s="6"/>
+      <c r="A157" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B157" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B158" s="6" t="s">
+      <c r="B158" s="6"/>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B159" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C159" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C158" s="6" t="s">
+      <c r="D159" t="s">
         <v>18</v>
-      </c>
-      <c r="D158" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>1</v>
-      </c>
-      <c r="B159" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="C159" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="D159" t="s">
-        <v>5</v>
-      </c>
-      <c r="E159" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B160" s="6">
-        <v>0.99</v>
+        <v>0.15</v>
       </c>
       <c r="C160" s="6">
-        <v>0.99</v>
+        <v>0.15</v>
       </c>
       <c r="D160" t="s">
         <v>5</v>
       </c>
       <c r="E160" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B161" s="6">
-        <v>1E-3</v>
+        <v>0.99</v>
       </c>
       <c r="C161" s="6">
-        <v>1E-3</v>
+        <v>0.99</v>
       </c>
       <c r="D161" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E161" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="B162" s="6">
-        <v>100</v>
-      </c>
-      <c r="C162" s="6"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C162" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="D162" t="s">
+        <v>6</v>
+      </c>
+      <c r="E162" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B163" s="6">
-        <v>10</v>
-      </c>
-      <c r="C163" s="6">
-        <v>1</v>
-      </c>
-      <c r="D163" t="s">
-        <v>87</v>
-      </c>
-      <c r="E163" t="s">
-        <v>88</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C163" s="6"/>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>0</v>
-      </c>
-      <c r="B164" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C164" s="6" t="s">
-        <v>0</v>
+        <v>85</v>
+      </c>
+      <c r="B164" s="6">
+        <v>10</v>
+      </c>
+      <c r="C164" s="6">
+        <v>1</v>
+      </c>
+      <c r="D164" t="s">
+        <v>86</v>
       </c>
       <c r="E164" t="s">
-        <v>0</v>
+        <v>87</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>64</v>
-      </c>
-      <c r="B165" s="6">
-        <v>3600</v>
-      </c>
-      <c r="C165" s="6">
-        <v>3600</v>
-      </c>
-      <c r="D165" t="s">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="B165" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C165" s="6" t="s">
+        <v>0</v>
       </c>
       <c r="E165" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B166" s="6">
+        <v>3600</v>
+      </c>
+      <c r="C166" s="6">
+        <v>3600</v>
+      </c>
+      <c r="D166" t="s">
+        <v>7</v>
+      </c>
+      <c r="E166" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>64</v>
+      </c>
+      <c r="B167" s="6">
         <v>50000</v>
       </c>
-      <c r="C166" s="6">
+      <c r="C167" s="6">
         <v>50000</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D167" t="s">
         <v>8</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E167" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B167" s="6"/>
-      <c r="C167" s="6"/>
-    </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>83</v>
-      </c>
-      <c r="B168" s="6">
-        <v>3</v>
-      </c>
+      <c r="B168" s="6"/>
       <c r="C168" s="6"/>
-      <c r="E168" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>43</v>
-      </c>
-      <c r="B169" s="6"/>
+        <v>82</v>
+      </c>
+      <c r="B169" s="6">
+        <v>3</v>
+      </c>
       <c r="C169" s="6"/>
+      <c r="E169" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>42</v>
+      </c>
       <c r="B170" s="6"/>
+      <c r="C170" s="6"/>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B171" s="6"/>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A172" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="B172" s="6"/>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A173" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B173" s="7" t="s">
-        <v>16</v>
+      <c r="A173" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B174" s="7">
-        <v>1</v>
+        <v>153</v>
+      </c>
+      <c r="B174" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B175" s="6"/>
+      <c r="A175" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B175" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B176" s="6" t="s">
+      <c r="B176" s="6"/>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B177" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C177" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C176" s="6" t="s">
+      <c r="D177" t="s">
         <v>18</v>
-      </c>
-      <c r="D176" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>1</v>
-      </c>
-      <c r="B177" s="6">
-        <v>0.08</v>
-      </c>
-      <c r="C177" s="6">
-        <v>0.08</v>
-      </c>
-      <c r="D177" t="s">
-        <v>5</v>
-      </c>
-      <c r="E177" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>113</v>
+        <v>1</v>
       </c>
       <c r="B178" s="6">
-        <v>2</v>
-      </c>
-      <c r="C178" s="6" t="s">
-        <v>114</v>
+        <v>0.08</v>
+      </c>
+      <c r="C178" s="6">
+        <v>0.08</v>
       </c>
       <c r="D178" t="s">
-        <v>115</v>
+        <v>5</v>
       </c>
       <c r="E178" t="s">
-        <v>116</v>
+        <v>9</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
+        <v>112</v>
+      </c>
+      <c r="B179" s="6">
         <v>2</v>
       </c>
-      <c r="B179" s="6">
-        <v>0.99</v>
-      </c>
-      <c r="C179" s="6">
-        <v>0.99</v>
+      <c r="C179" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="D179" t="s">
-        <v>5</v>
+        <v>114</v>
       </c>
       <c r="E179" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B180" s="6">
-        <v>1E-3</v>
+        <v>0.99</v>
       </c>
       <c r="C180" s="6">
-        <v>1E-3</v>
+        <v>0.99</v>
       </c>
       <c r="D180" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E180" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="B181" s="6">
-        <v>0</v>
-      </c>
-      <c r="C181" s="6"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C181" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="D181" t="s">
+        <v>6</v>
+      </c>
+      <c r="E181" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B182" s="6">
-        <v>10</v>
-      </c>
-      <c r="C182" s="6">
-        <v>1</v>
-      </c>
-      <c r="D182" t="s">
-        <v>87</v>
-      </c>
-      <c r="E182" t="s">
-        <v>88</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C182" s="6"/>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>0</v>
-      </c>
-      <c r="B183" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C183" s="6" t="s">
-        <v>0</v>
+        <v>85</v>
+      </c>
+      <c r="B183" s="6">
+        <v>10</v>
+      </c>
+      <c r="C183" s="6">
+        <v>1</v>
+      </c>
+      <c r="D183" t="s">
+        <v>86</v>
       </c>
       <c r="E183" t="s">
-        <v>0</v>
+        <v>87</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>64</v>
-      </c>
-      <c r="B184" s="6">
-        <v>3600</v>
-      </c>
-      <c r="C184" s="6">
-        <v>3600</v>
-      </c>
-      <c r="D184" t="s">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="B184" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C184" s="6" t="s">
+        <v>0</v>
       </c>
       <c r="E184" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B185" s="6">
+        <v>3600</v>
+      </c>
+      <c r="C185" s="6">
+        <v>3600</v>
+      </c>
+      <c r="D185" t="s">
+        <v>7</v>
+      </c>
+      <c r="E185" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>64</v>
+      </c>
+      <c r="B186" s="6">
         <v>50000</v>
       </c>
-      <c r="C185" s="6">
+      <c r="C186" s="6">
         <v>50000</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D186" t="s">
         <v>8</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E186" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B186" s="6"/>
-      <c r="C186" s="6"/>
-    </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>117</v>
-      </c>
-      <c r="B187" s="4" t="s">
-        <v>118</v>
-      </c>
+      <c r="B187" s="6"/>
       <c r="C187" s="6"/>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>43</v>
-      </c>
-      <c r="B188" s="6"/>
+        <v>116</v>
+      </c>
+      <c r="B188" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C188" s="6"/>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>42</v>
+      </c>
       <c r="B189" s="6"/>
-      <c r="C189" s="6"/>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B190" s="9"/>
+      <c r="B190" s="6"/>
       <c r="C190" s="6"/>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B191" s="6"/>
+      <c r="B191" s="9"/>
       <c r="C191" s="6"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B192" s="6"/>
-      <c r="C192" s="6"/>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B193" s="6"/>
+      <c r="A192" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B193" t="s">
+        <v>15</v>
+      </c>
       <c r="C193" s="6"/>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B194" s="6"/>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B194" s="6">
+        <v>1</v>
+      </c>
       <c r="C194" s="6"/>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B195" s="6"/>
       <c r="C195" s="6"/>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B196" s="6"/>
-      <c r="C196" s="6"/>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B197" s="6"/>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B196" t="s">
+        <v>16</v>
+      </c>
+      <c r="C196" t="s">
+        <v>17</v>
+      </c>
+      <c r="D196" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>156</v>
+      </c>
+      <c r="B197" s="6">
+        <v>20</v>
+      </c>
       <c r="C197" s="6"/>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B198" s="6"/>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A199" s="2"/>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A200" s="2"/>
-    </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B214" s="9"/>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>157</v>
+      </c>
+      <c r="B198" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C198" s="6"/>
+      <c r="E198" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>159</v>
+      </c>
+      <c r="B199" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="C199" s="6"/>
+      <c r="E199" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>161</v>
+      </c>
+      <c r="B200" s="6">
+        <v>3</v>
+      </c>
+      <c r="C200" s="6"/>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>162</v>
+      </c>
+      <c r="B201" s="6">
+        <v>1</v>
+      </c>
+      <c r="C201" s="6"/>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>42</v>
+      </c>
+      <c r="B202" s="6"/>
+      <c r="C202" s="6"/>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B207">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B209" t="s">
+        <v>16</v>
+      </c>
+      <c r="C209" t="s">
+        <v>17</v>
+      </c>
+      <c r="D209" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B213" s="9"/>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C215" s="6"/>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B216" s="6">
+        <v>1</v>
+      </c>
+      <c r="C216" s="6"/>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B217" s="6"/>
+      <c r="C217" s="6"/>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B218" t="s">
+        <v>16</v>
+      </c>
+      <c r="C218" t="s">
+        <v>17</v>
+      </c>
+      <c r="D218" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B219">
+        <v>0.25</v>
+      </c>
+      <c r="C219" s="6"/>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>42</v>
+      </c>
+      <c r="B220" s="6"/>
+      <c r="C220" s="6"/>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" s="1"/>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" s="2"/>
+      <c r="B222" s="7"/>
+      <c r="C222" s="6"/>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C224" s="6"/>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B225" s="6">
+        <v>1</v>
+      </c>
+      <c r="C225" s="6"/>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B226" s="6"/>
+      <c r="C226" s="6"/>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B227" t="s">
+        <v>16</v>
+      </c>
+      <c r="C227" t="s">
+        <v>17</v>
+      </c>
+      <c r="D227" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B228">
+        <v>0.05</v>
+      </c>
+      <c r="C228" s="6"/>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>42</v>
+      </c>
+      <c r="B229" s="6"/>
+      <c r="C229" s="6"/>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" s="4"/>
+      <c r="C241" s="6"/>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A242" s="4"/>
-      <c r="C242" s="6"/>
+      <c r="A242" s="1"/>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A243" s="1"/>
+      <c r="A243" s="2"/>
+      <c r="B243" s="7"/>
+      <c r="C243" s="6"/>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" s="2"/>
@@ -2606,8 +2875,7 @@
       <c r="C244" s="6"/>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A245" s="2"/>
-      <c r="B245" s="7"/>
+      <c r="B245" s="6"/>
       <c r="C245" s="6"/>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
@@ -2686,18 +2954,19 @@
       <c r="B264" s="6"/>
       <c r="C264" s="6"/>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B265" s="6"/>
-      <c r="C265" s="6"/>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B267" s="6"/>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B268" s="6"/>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B269" s="6"/>
+      <c r="A269" s="1"/>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A270" s="1"/>
+      <c r="A270" s="2"/>
+      <c r="B270" s="7"/>
+      <c r="C270" s="6"/>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" s="2"/>
@@ -2705,8 +2974,7 @@
       <c r="C271" s="6"/>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A272" s="2"/>
-      <c r="B272" s="7"/>
+      <c r="B272" s="6"/>
       <c r="C272" s="6"/>
     </row>
     <row r="273" spans="2:3" x14ac:dyDescent="0.25">
@@ -2758,11 +3026,7 @@
       <c r="C284" s="6"/>
     </row>
     <row r="285" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B285" s="6"/>
       <c r="C285" s="6"/>
-    </row>
-    <row r="286" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C286" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updates in main file
</commit_message>
<xml_diff>
--- a/results/peat_suossjavri/peat_suossjavri.xlsx
+++ b/results/peat_suossjavri/peat_suossjavri.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\thin\02_Code\Matlab\CryoGRID\202008_CryoGrid_NewOOP_GIT - CURRENT_THIN\results\peat_suossjavri\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\git\CryoGrid\results\peat_suossjavri\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -278,9 +278,6 @@
     <t>not used,</t>
   </si>
   <si>
-    <t>OUT_all</t>
-  </si>
-  <si>
     <t>area</t>
   </si>
   <si>
@@ -525,6 +522,9 @@
   </si>
   <si>
     <t>LATERAL_IA_CLASS</t>
+  </si>
+  <si>
+    <t>OUT_all_lateral</t>
   </si>
 </sst>
 </file>
@@ -869,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="A193" sqref="A193"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,13 +889,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
@@ -903,152 +903,152 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
         <v>122</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>123</v>
-      </c>
-      <c r="D4" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" t="s">
         <v>125</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>126</v>
-      </c>
-      <c r="D5" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" t="s">
         <v>128</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>129</v>
-      </c>
-      <c r="D6" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" t="s">
         <v>131</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>132</v>
-      </c>
-      <c r="D7" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
         <v>134</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
         <v>136</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
         <v>138</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
         <v>140</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
         <v>142</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
         <v>144</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" t="s">
         <v>148</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>149</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>150</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>151</v>
-      </c>
-      <c r="E14" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B15">
         <v>0.25</v>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1072,7 +1072,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>84</v>
+        <v>166</v>
       </c>
       <c r="B20" s="2">
         <v>1</v>
@@ -1145,7 +1145,7 @@
         <v>50</v>
       </c>
       <c r="B31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1170,7 +1170,7 @@
         <v>51</v>
       </c>
       <c r="B34">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
@@ -1184,7 +1184,7 @@
         <v>52</v>
       </c>
       <c r="B35">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B67">
         <v>0.5</v>
@@ -1503,7 +1503,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B68">
         <v>0.5</v>
@@ -1552,10 +1552,10 @@
         <v>24</v>
       </c>
       <c r="B76" t="s">
+        <v>88</v>
+      </c>
+      <c r="C76" t="s">
         <v>89</v>
-      </c>
-      <c r="C76" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -1573,7 +1573,7 @@
         <v>0</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -1584,7 +1584,7 @@
         <v>10</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -1601,16 +1601,16 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C83" s="8"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B84" s="4">
         <v>1</v>
@@ -1723,7 +1723,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B105" s="7" t="s">
         <v>15</v>
@@ -1732,7 +1732,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B106" s="7">
         <v>1</v>
@@ -1807,7 +1807,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B112" s="6">
         <v>100</v>
@@ -1816,19 +1816,19 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>84</v>
+      </c>
+      <c r="B113" s="6">
+        <v>1</v>
+      </c>
+      <c r="C113" s="6">
+        <v>1</v>
+      </c>
+      <c r="D113" t="s">
         <v>85</v>
       </c>
-      <c r="B113" s="6">
-        <v>1</v>
-      </c>
-      <c r="C113" s="6">
-        <v>1</v>
-      </c>
-      <c r="D113" t="s">
+      <c r="E113" t="s">
         <v>86</v>
-      </c>
-      <c r="E113" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -1837,7 +1837,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B115" s="9">
         <v>1.0000000000000001E-5</v>
@@ -1846,7 +1846,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B116">
         <v>0.1</v>
@@ -1855,7 +1855,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B117">
         <v>0.1</v>
@@ -1864,7 +1864,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B118">
         <v>0.5</v>
@@ -1877,7 +1877,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B120" s="6">
         <v>1000</v>
@@ -1886,7 +1886,7 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B121" s="6">
         <v>1000</v>
@@ -1895,7 +1895,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B122" s="6">
         <v>-40</v>
@@ -1909,7 +1909,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B123" s="6">
         <v>0.05</v>
@@ -1926,7 +1926,7 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B124" s="6">
         <v>0.97</v>
@@ -1943,7 +1943,7 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B125" s="6">
         <v>0.03</v>
@@ -1982,7 +1982,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B129" s="6">
         <v>0.01</v>
@@ -2021,7 +2021,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B135" s="7" t="s">
         <v>15</v>
@@ -2030,7 +2030,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B136" s="7">
         <v>1</v>
@@ -2057,7 +2057,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B139" s="6">
         <v>0</v>
@@ -2074,7 +2074,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B140" s="6">
         <v>0.71</v>
@@ -2083,14 +2083,14 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B141" s="6">
         <v>0.21</v>
       </c>
       <c r="C141" s="6"/>
       <c r="D141" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -2113,7 +2113,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B144" s="6">
         <v>0</v>
@@ -2122,7 +2122,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B145" s="6">
         <v>48</v>
@@ -2156,7 +2156,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B147" s="9">
         <v>1E-4</v>
@@ -2165,7 +2165,7 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B148" s="6">
         <v>0.02</v>
@@ -2214,7 +2214,7 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B156" s="7" t="s">
         <v>15</v>
@@ -2222,7 +2222,7 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B157" s="7">
         <v>1</v>
@@ -2295,7 +2295,7 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B163" s="6">
         <v>100</v>
@@ -2304,7 +2304,7 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B164" s="6">
         <v>10</v>
@@ -2313,10 +2313,10 @@
         <v>1</v>
       </c>
       <c r="D164" t="s">
+        <v>85</v>
+      </c>
+      <c r="E164" t="s">
         <v>86</v>
-      </c>
-      <c r="E164" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -2403,7 +2403,7 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B174" s="7" t="s">
         <v>15</v>
@@ -2411,7 +2411,7 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B175" s="7">
         <v>1</v>
@@ -2450,19 +2450,19 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B179" s="6">
         <v>2</v>
       </c>
       <c r="C179" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D179" t="s">
         <v>113</v>
       </c>
-      <c r="D179" t="s">
+      <c r="E179" t="s">
         <v>114</v>
-      </c>
-      <c r="E179" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -2501,7 +2501,7 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B182" s="6">
         <v>0</v>
@@ -2510,7 +2510,7 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B183" s="6">
         <v>10</v>
@@ -2519,10 +2519,10 @@
         <v>1</v>
       </c>
       <c r="D183" t="s">
+        <v>85</v>
+      </c>
+      <c r="E183" t="s">
         <v>86</v>
-      </c>
-      <c r="E183" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
@@ -2579,10 +2579,10 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
+        <v>115</v>
+      </c>
+      <c r="B188" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="B188" s="4" t="s">
-        <v>117</v>
       </c>
       <c r="C188" s="6"/>
     </row>
@@ -2607,7 +2607,7 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B193" t="s">
         <v>15</v>
@@ -2616,7 +2616,7 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B194" s="6">
         <v>1</v>
@@ -2640,7 +2640,7 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B197" s="6">
         <v>20</v>
@@ -2649,31 +2649,31 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B198" s="6">
         <v>0.5</v>
       </c>
       <c r="C198" s="6"/>
       <c r="E198" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B199" s="6">
         <v>0.03</v>
       </c>
       <c r="C199" s="6"/>
       <c r="E199" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B200" s="6">
         <v>3</v>
@@ -2682,7 +2682,7 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B201" s="6">
         <v>1</v>
@@ -2703,7 +2703,7 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B206" s="2" t="s">
         <v>15</v>
@@ -2711,7 +2711,7 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B207">
         <v>1</v>
@@ -2730,7 +2730,7 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -2748,7 +2748,7 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B215" s="2" t="s">
         <v>15</v>
@@ -2757,7 +2757,7 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B216" s="6">
         <v>1</v>
@@ -2781,7 +2781,7 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B219">
         <v>0.25</v>
@@ -2810,7 +2810,7 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B224" s="2" t="s">
         <v>15</v>
@@ -2819,7 +2819,7 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B225" s="6">
         <v>1</v>
@@ -2843,7 +2843,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B228">
         <v>0.05</v>

</xml_diff>

<commit_message>
update druing final cleanup
</commit_message>
<xml_diff>
--- a/results/peat_suossjavri/peat_suossjavri.xlsx
+++ b/results/peat_suossjavri/peat_suossjavri.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="172">
   <si>
     <t xml:space="preserve">    </t>
   </si>
@@ -494,9 +494,6 @@
     <t>reservoir_temperature</t>
   </si>
   <si>
-    <t>only active for Xice classes - if empty, water added at the temperature of the respective grid cell</t>
-  </si>
-  <si>
     <t>hardBottom_cutoff</t>
   </si>
   <si>
@@ -524,7 +521,25 @@
     <t>LATERAL_IA_CLASS</t>
   </si>
   <si>
-    <t>OUT_all_lateral</t>
+    <t>if empty, water is added at grid cell temperature</t>
+  </si>
+  <si>
+    <t>LAT_SEEPAGE_FACE_WATER</t>
+  </si>
+  <si>
+    <t>upperElevation</t>
+  </si>
+  <si>
+    <t>lowerElevation</t>
+  </si>
+  <si>
+    <t>distance_seepageFace</t>
+  </si>
+  <si>
+    <t>seepage_contact_length</t>
+  </si>
+  <si>
+    <t>OUT_all</t>
   </si>
 </sst>
 </file>
@@ -867,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F285"/>
+  <dimension ref="A1:F297"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,8 +1051,8 @@
       <c r="B14" t="s">
         <v>148</v>
       </c>
-      <c r="C14" t="s">
-        <v>149</v>
+      <c r="C14" s="4" t="s">
+        <v>166</v>
       </c>
       <c r="D14" t="s">
         <v>150</v>
@@ -1072,7 +1087,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="B20" s="2">
         <v>1</v>
@@ -2607,7 +2622,7 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B193" t="s">
         <v>15</v>
@@ -2643,7 +2658,7 @@
         <v>154</v>
       </c>
       <c r="B197" s="6">
-        <v>20</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="C197" s="6"/>
     </row>
@@ -2651,29 +2666,27 @@
       <c r="A198" t="s">
         <v>155</v>
       </c>
-      <c r="B198" s="6">
-        <v>0.5</v>
-      </c>
+      <c r="B198" s="6"/>
       <c r="C198" s="6"/>
       <c r="E198" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B199" s="6">
         <v>0.03</v>
       </c>
       <c r="C199" s="6"/>
       <c r="E199" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B200" s="6">
         <v>3</v>
@@ -2682,7 +2695,7 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B201" s="6">
         <v>1</v>
@@ -2696,6 +2709,10 @@
       <c r="B202" s="6"/>
       <c r="C202" s="6"/>
     </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B203" s="6"/>
+      <c r="C203" s="6"/>
+    </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>23</v>
@@ -2703,19 +2720,25 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B206" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B206" t="s">
         <v>15</v>
       </c>
+      <c r="C206" s="6"/>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B207">
-        <v>1</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="B207" s="6">
+        <v>1</v>
+      </c>
+      <c r="C207" s="6"/>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B208" s="6"/>
+      <c r="C208" s="6"/>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
@@ -2730,303 +2753,387 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>161</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="B210" s="6">
+        <v>100000</v>
+      </c>
+      <c r="C210" s="6"/>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
+        <v>168</v>
+      </c>
+      <c r="B211" s="6">
+        <v>15</v>
+      </c>
+      <c r="C211" s="6"/>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>156</v>
+      </c>
+      <c r="B212" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="C212" s="6"/>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>169</v>
+      </c>
+      <c r="B213" s="6">
+        <v>3</v>
+      </c>
+      <c r="C213" s="6"/>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>170</v>
+      </c>
+      <c r="B214" s="6">
+        <v>1</v>
+      </c>
+      <c r="C214" s="6"/>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B213" s="9"/>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" s="1" t="s">
+      <c r="B215" s="6"/>
+      <c r="C215" s="6"/>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B215" s="2" t="s">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B218" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C215" s="6"/>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B216" s="6">
-        <v>1</v>
-      </c>
-      <c r="C216" s="6"/>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B217" s="6"/>
-      <c r="C217" s="6"/>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B218" t="s">
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B221" t="s">
         <v>16</v>
       </c>
-      <c r="C218" t="s">
+      <c r="C221" t="s">
         <v>17</v>
       </c>
-      <c r="D218" t="s">
+      <c r="D221" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A219" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="B219">
-        <v>0.25</v>
-      </c>
-      <c r="C219" s="6"/>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
         <v>42</v>
       </c>
-      <c r="B220" s="6"/>
-      <c r="C220" s="6"/>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A221" s="1"/>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A222" s="2"/>
-      <c r="B222" s="7"/>
-      <c r="C222" s="6"/>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A223" s="1" t="s">
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B225" s="9"/>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A224" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B224" s="2" t="s">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B227" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C224" s="6"/>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A225" s="2" t="s">
+      <c r="C227" s="6"/>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B225" s="6">
-        <v>1</v>
-      </c>
-      <c r="C225" s="6"/>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B226" s="6"/>
-      <c r="C226" s="6"/>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B227" t="s">
-        <v>16</v>
-      </c>
-      <c r="C227" t="s">
-        <v>17</v>
-      </c>
-      <c r="D227" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A228" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="B228">
-        <v>0.05</v>
+      <c r="B228" s="6">
+        <v>1</v>
       </c>
       <c r="C228" s="6"/>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" t="s">
-        <v>42</v>
-      </c>
       <c r="B229" s="6"/>
       <c r="C229" s="6"/>
     </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B230" t="s">
+        <v>16</v>
+      </c>
+      <c r="C230" t="s">
+        <v>17</v>
+      </c>
+      <c r="D230" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B231">
+        <v>0.25</v>
+      </c>
+      <c r="C231" s="6"/>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>42</v>
+      </c>
+      <c r="B232" s="6"/>
+      <c r="C232" s="6"/>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" s="1"/>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" s="2"/>
+      <c r="B234" s="7"/>
+      <c r="C234" s="6"/>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C236" s="6"/>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A237" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B237" s="6">
+        <v>1</v>
+      </c>
+      <c r="C237" s="6"/>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B238" s="6"/>
+      <c r="C238" s="6"/>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B239" t="s">
+        <v>16</v>
+      </c>
+      <c r="C239" t="s">
+        <v>17</v>
+      </c>
+      <c r="D239" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A240" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B240">
+        <v>0.05</v>
+      </c>
+      <c r="C240" s="6"/>
+    </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A241" s="4"/>
+      <c r="A241" t="s">
+        <v>42</v>
+      </c>
+      <c r="B241" s="6"/>
       <c r="C241" s="6"/>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A242" s="1"/>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A243" s="2"/>
-      <c r="B243" s="7"/>
-      <c r="C243" s="6"/>
-    </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A244" s="2"/>
-      <c r="B244" s="7"/>
-      <c r="C244" s="6"/>
-    </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B245" s="6"/>
-      <c r="C245" s="6"/>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B246" s="6"/>
-      <c r="C246" s="6"/>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B247" s="6"/>
-      <c r="C247" s="6"/>
-    </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B248" s="6"/>
-      <c r="C248" s="6"/>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B249" s="6"/>
-      <c r="C249" s="6"/>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B250" s="6"/>
-      <c r="C250" s="6"/>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B251" s="6"/>
-      <c r="C251" s="6"/>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B252" s="6"/>
-      <c r="C252" s="6"/>
-    </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B253" s="6"/>
+      <c r="A253" s="4"/>
       <c r="C253" s="6"/>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B254" s="6"/>
-      <c r="C254" s="6"/>
+      <c r="A254" s="1"/>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B255" s="6"/>
+      <c r="A255" s="2"/>
+      <c r="B255" s="7"/>
       <c r="C255" s="6"/>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B256" s="6"/>
+      <c r="A256" s="2"/>
+      <c r="B256" s="7"/>
       <c r="C256" s="6"/>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B257" s="6"/>
       <c r="C257" s="6"/>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B258" s="6"/>
       <c r="C258" s="6"/>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B259" s="6"/>
       <c r="C259" s="6"/>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B260" s="6"/>
       <c r="C260" s="6"/>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B261" s="6"/>
       <c r="C261" s="6"/>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B262" s="6"/>
       <c r="C262" s="6"/>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B263" s="6"/>
       <c r="C263" s="6"/>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B264" s="6"/>
       <c r="C264" s="6"/>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B265" s="6"/>
+      <c r="C265" s="6"/>
+    </row>
+    <row r="266" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B266" s="6"/>
+      <c r="C266" s="6"/>
+    </row>
+    <row r="267" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B267" s="6"/>
-    </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C267" s="6"/>
+    </row>
+    <row r="268" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B268" s="6"/>
-    </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A269" s="1"/>
-    </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A270" s="2"/>
-      <c r="B270" s="7"/>
+      <c r="C268" s="6"/>
+    </row>
+    <row r="269" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B269" s="6"/>
+      <c r="C269" s="6"/>
+    </row>
+    <row r="270" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B270" s="6"/>
       <c r="C270" s="6"/>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A271" s="2"/>
-      <c r="B271" s="7"/>
+    <row r="271" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B271" s="6"/>
       <c r="C271" s="6"/>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B272" s="6"/>
       <c r="C272" s="6"/>
     </row>
-    <row r="273" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B273" s="6"/>
       <c r="C273" s="6"/>
     </row>
-    <row r="274" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B274" s="6"/>
       <c r="C274" s="6"/>
     </row>
-    <row r="275" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B275" s="6"/>
       <c r="C275" s="6"/>
     </row>
-    <row r="276" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B276" s="6"/>
       <c r="C276" s="6"/>
     </row>
-    <row r="277" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B277" s="6"/>
-      <c r="C277" s="6"/>
-    </row>
-    <row r="278" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B278" s="6"/>
-      <c r="C278" s="6"/>
-    </row>
-    <row r="279" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B279" s="6"/>
-      <c r="C279" s="6"/>
-    </row>
-    <row r="280" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B280" s="6"/>
-      <c r="C280" s="6"/>
-    </row>
-    <row r="281" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B281" s="6"/>
-      <c r="C281" s="6"/>
-    </row>
-    <row r="282" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B282" s="6"/>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281" s="1"/>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A282" s="2"/>
+      <c r="B282" s="7"/>
       <c r="C282" s="6"/>
     </row>
-    <row r="283" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B283" s="6"/>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283" s="2"/>
+      <c r="B283" s="7"/>
       <c r="C283" s="6"/>
     </row>
-    <row r="284" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B284" s="6"/>
       <c r="C284" s="6"/>
     </row>
-    <row r="285" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B285" s="6"/>
       <c r="C285" s="6"/>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B286" s="6"/>
+      <c r="C286" s="6"/>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B287" s="6"/>
+      <c r="C287" s="6"/>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B288" s="6"/>
+      <c r="C288" s="6"/>
+    </row>
+    <row r="289" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B289" s="6"/>
+      <c r="C289" s="6"/>
+    </row>
+    <row r="290" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B290" s="6"/>
+      <c r="C290" s="6"/>
+    </row>
+    <row r="291" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B291" s="6"/>
+      <c r="C291" s="6"/>
+    </row>
+    <row r="292" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B292" s="6"/>
+      <c r="C292" s="6"/>
+    </row>
+    <row r="293" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B293" s="6"/>
+      <c r="C293" s="6"/>
+    </row>
+    <row r="294" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B294" s="6"/>
+      <c r="C294" s="6"/>
+    </row>
+    <row r="295" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B295" s="6"/>
+      <c r="C295" s="6"/>
+    </row>
+    <row r="296" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B296" s="6"/>
+      <c r="C296" s="6"/>
+    </row>
+    <row r="297" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C297" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>